<commit_message>
reading excel to array
</commit_message>
<xml_diff>
--- a/src/test/resources/test_data/Hrm_data.xlsx
+++ b/src/test/resources/test_data/Hrm_data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\eclipse-workspace\HealthManagementAutomation\src\test\resources\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
   <si>
     <t xml:space="preserve">username </t>
   </si>
@@ -48,6 +48,15 @@
   </si>
   <si>
     <t>peter123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Admin </t>
+  </si>
+  <si>
+    <t>Admin321</t>
+  </si>
+  <si>
+    <t>abhi</t>
   </si>
 </sst>
 </file>
@@ -377,10 +386,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -423,6 +432,28 @@
         <v>5</v>
       </c>
     </row>
+    <row r="4" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5">
+        <v>1234</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Sending testdata through excel
</commit_message>
<xml_diff>
--- a/src/test/resources/test_data/Hrm_data.xlsx
+++ b/src/test/resources/test_data/Hrm_data.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="invalidLogin" sheetId="1" r:id="rId1"/>
+    <sheet name="validLogin" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="15">
   <si>
     <t xml:space="preserve">username </t>
   </si>
@@ -57,6 +58,18 @@
   </si>
   <si>
     <t>abhi</t>
+  </si>
+  <si>
+    <t>expectedHeader</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>admin123</t>
+  </si>
+  <si>
+    <t>Dashboard</t>
   </si>
 </sst>
 </file>
@@ -388,8 +401,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -458,4 +471,52 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>